<commit_message>
27 - Analyse maken ( https://italent.cloudapp.net:9443/ccm/web/projects/iTalent#action=com.ibm.team.workitem.viewWorkItem&id=27 )
</commit_message>
<xml_diff>
--- a/italent/documents/analyse/Gegroepeerde use cases.xlsx
+++ b/italent/documents/analyse/Gegroepeerde use cases.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkspaceITalent\italent\documents\analyse\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22275" windowHeight="8700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19095" windowHeight="8205"/>
   </bookViews>
   <sheets>
     <sheet name="Gebeurtenissen" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -362,7 +358,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -406,9 +402,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -446,7 +442,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -518,7 +514,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -671,7 +667,7 @@
   <dimension ref="B1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,7 +697,7 @@
       <c r="K2" s="26"/>
     </row>
     <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
@@ -716,22 +712,6 @@
       </c>
       <c r="F5" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="H5" s="21">
-        <f t="shared" ref="H5:H23" si="0">B6</f>
-        <v>1</v>
-      </c>
-      <c r="I5" s="13" t="str">
-        <f t="shared" ref="I5:I23" si="1">IF(D6="x",LOWER($D$5),"")&amp;IF(E6="x",", " &amp; LOWER($E$5),"")&amp;IF(F6="x", ", " &amp; LOWER($F$5),"") &amp; " kunnen " &amp; LOWER(C6)</f>
-        <v>studenten, docenten kunnen inloggen</v>
-      </c>
-      <c r="J5" s="13" t="str">
-        <f>IF(LEFT(I5,1)=",",MID(I5,3,LEN(I5)),I5)</f>
-        <v>studenten, docenten kunnen inloggen</v>
-      </c>
-      <c r="K5" s="14" t="str">
-        <f>UPPER(LEFT(J5,1))&amp;LOWER(RIGHT(J5,LEN(J5)-1))</f>
-        <v>Studenten, docenten kunnen inloggen</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
@@ -748,21 +728,21 @@
         <v>5</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="H6" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I6" s="19" t="str">
-        <f t="shared" si="1"/>
-        <v>studenten, docenten, gasten kunnen projectenlijst bekijken</v>
-      </c>
-      <c r="J6" s="19" t="str">
-        <f t="shared" ref="J6:J10" si="2">IF(LEFT(I6,1)=",",MID(I6,3,LEN(I6)),I6)</f>
-        <v>studenten, docenten, gasten kunnen projectenlijst bekijken</v>
-      </c>
-      <c r="K6" s="20" t="str">
-        <f t="shared" ref="K6:K23" si="3">UPPER(LEFT(J6,1))&amp;LOWER(RIGHT(J6,LEN(J6)-1))</f>
-        <v>Studenten, docenten, gasten kunnen projectenlijst bekijken</v>
+      <c r="H6" s="21">
+        <f>B6</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="13" t="str">
+        <f>IF(D6="x",LOWER($D$5),"")&amp;IF(E6="x",", " &amp; LOWER($E$5),"")&amp;IF(F6="x", ", " &amp; LOWER($F$5),"") &amp; " kunnen " &amp; LOWER(C6)</f>
+        <v>studenten, docenten kunnen inloggen</v>
+      </c>
+      <c r="J6" s="13" t="str">
+        <f>IF(LEFT(I6,1)=",",MID(I6,3,LEN(I6)),I6)</f>
+        <v>studenten, docenten kunnen inloggen</v>
+      </c>
+      <c r="K6" s="14" t="str">
+        <f>UPPER(LEFT(J6,1))&amp;LOWER(RIGHT(J6,LEN(J6)-1))</f>
+        <v>Studenten, docenten kunnen inloggen</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
@@ -781,21 +761,21 @@
       <c r="F7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="22">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I7" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v>studenten, docenten, gasten kunnen projectenlijst sorteren</v>
-      </c>
-      <c r="J7" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v>studenten, docenten, gasten kunnen projectenlijst sorteren</v>
-      </c>
-      <c r="K7" s="16" t="str">
-        <f t="shared" si="3"/>
-        <v>Studenten, docenten, gasten kunnen projectenlijst sorteren</v>
+      <c r="H7" s="11">
+        <f>B7</f>
+        <v>2</v>
+      </c>
+      <c r="I7" s="19" t="str">
+        <f>IF(D7="x",LOWER($D$5),"")&amp;IF(E7="x",", " &amp; LOWER($E$5),"")&amp;IF(F7="x", ", " &amp; LOWER($F$5),"") &amp; " kunnen " &amp; LOWER(C7)</f>
+        <v>studenten, docenten, gasten kunnen projectenlijst bekijken</v>
+      </c>
+      <c r="J7" s="19" t="str">
+        <f t="shared" ref="J7:J11" si="0">IF(LEFT(I7,1)=",",MID(I7,3,LEN(I7)),I7)</f>
+        <v>studenten, docenten, gasten kunnen projectenlijst bekijken</v>
+      </c>
+      <c r="K7" s="20" t="str">
+        <f t="shared" ref="K7:K24" si="1">UPPER(LEFT(J7,1))&amp;LOWER(RIGHT(J7,LEN(J7)-1))</f>
+        <v>Studenten, docenten, gasten kunnen projectenlijst bekijken</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
@@ -814,21 +794,21 @@
       <c r="F8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="22">
+        <f>B8</f>
+        <v>3</v>
+      </c>
+      <c r="I8" s="15" t="str">
+        <f>IF(D8="x",LOWER($D$5),"")&amp;IF(E8="x",", " &amp; LOWER($E$5),"")&amp;IF(F8="x", ", " &amp; LOWER($F$5),"") &amp; " kunnen " &amp; LOWER(C8)</f>
+        <v>studenten, docenten, gasten kunnen projectenlijst sorteren</v>
+      </c>
+      <c r="J8" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="I8" s="19" t="str">
-        <f t="shared" si="1"/>
-        <v>studenten, docenten, gasten kunnen projecten filteren</v>
-      </c>
-      <c r="J8" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>studenten, docenten, gasten kunnen projecten filteren</v>
-      </c>
-      <c r="K8" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v>Studenten, docenten, gasten kunnen projecten filteren</v>
+        <v>studenten, docenten, gasten kunnen projectenlijst sorteren</v>
+      </c>
+      <c r="K8" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>Studenten, docenten, gasten kunnen projectenlijst sorteren</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
@@ -847,21 +827,21 @@
       <c r="F9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H9" s="11">
+        <f>B9</f>
+        <v>4</v>
+      </c>
+      <c r="I9" s="19" t="str">
+        <f>IF(D9="x",LOWER($D$5),"")&amp;IF(E9="x",", " &amp; LOWER($E$5),"")&amp;IF(F9="x", ", " &amp; LOWER($F$5),"") &amp; " kunnen " &amp; LOWER(C9)</f>
+        <v>studenten, docenten, gasten kunnen projecten filteren</v>
+      </c>
+      <c r="J9" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="I9" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v>studenten, docenten, gasten kunnen projecten zoeken</v>
-      </c>
-      <c r="J9" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v>studenten, docenten, gasten kunnen projecten zoeken</v>
-      </c>
-      <c r="K9" s="16" t="str">
-        <f t="shared" si="3"/>
-        <v>Studenten, docenten, gasten kunnen projecten zoeken</v>
+        <v>studenten, docenten, gasten kunnen projecten filteren</v>
+      </c>
+      <c r="K9" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Studenten, docenten, gasten kunnen projecten filteren</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
@@ -880,21 +860,21 @@
       <c r="F10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="22">
+        <f>B10</f>
+        <v>5</v>
+      </c>
+      <c r="I10" s="15" t="str">
+        <f>IF(D10="x",LOWER($D$5),"")&amp;IF(E10="x",", " &amp; LOWER($E$5),"")&amp;IF(F10="x", ", " &amp; LOWER($F$5),"") &amp; " kunnen " &amp; LOWER(C10)</f>
+        <v>studenten, docenten, gasten kunnen projecten zoeken</v>
+      </c>
+      <c r="J10" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="I10" s="19" t="str">
-        <f t="shared" si="1"/>
-        <v>studenten, docenten kunnen projecten liken</v>
-      </c>
-      <c r="J10" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>studenten, docenten kunnen projecten liken</v>
-      </c>
-      <c r="K10" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v>Studenten, docenten kunnen projecten liken</v>
+        <v>studenten, docenten, gasten kunnen projecten zoeken</v>
+      </c>
+      <c r="K10" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>Studenten, docenten, gasten kunnen projecten zoeken</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
@@ -911,21 +891,21 @@
         <v>5</v>
       </c>
       <c r="F11" s="6"/>
-      <c r="H11" s="22">
+      <c r="H11" s="11">
+        <f>B11</f>
+        <v>6</v>
+      </c>
+      <c r="I11" s="19" t="str">
+        <f>IF(D11="x",LOWER($D$5),"")&amp;IF(E11="x",", " &amp; LOWER($E$5),"")&amp;IF(F11="x", ", " &amp; LOWER($F$5),"") &amp; " kunnen " &amp; LOWER(C11)</f>
+        <v>studenten, docenten kunnen projecten liken</v>
+      </c>
+      <c r="J11" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="I11" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v>studenten, docenten kunnen projectdetails opvragen</v>
-      </c>
-      <c r="J11" s="15" t="str">
-        <f>IF(LEFT(I11,1)=",",MID(I11,3,LEN(I11)),I11)</f>
-        <v>studenten, docenten kunnen projectdetails opvragen</v>
-      </c>
-      <c r="K11" s="16" t="str">
-        <f t="shared" si="3"/>
-        <v>Studenten, docenten kunnen projectdetails opvragen</v>
+        <v>studenten, docenten kunnen projecten liken</v>
+      </c>
+      <c r="K11" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Studenten, docenten kunnen projecten liken</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -942,21 +922,21 @@
         <v>5</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="H12" s="11">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="I12" s="19" t="str">
-        <f t="shared" si="1"/>
-        <v>studenten, docenten kunnen projectnieuws bekijken</v>
-      </c>
-      <c r="J12" s="19" t="str">
-        <f t="shared" ref="J12:J13" si="4">IF(LEFT(I12,1)=",",MID(I12,3,LEN(I12)),I12)</f>
-        <v>studenten, docenten kunnen projectnieuws bekijken</v>
-      </c>
-      <c r="K12" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v>Studenten, docenten kunnen projectnieuws bekijken</v>
+      <c r="H12" s="22">
+        <f>B12</f>
+        <v>7</v>
+      </c>
+      <c r="I12" s="15" t="str">
+        <f>IF(D12="x",LOWER($D$5),"")&amp;IF(E12="x",", " &amp; LOWER($E$5),"")&amp;IF(F12="x", ", " &amp; LOWER($F$5),"") &amp; " kunnen " &amp; LOWER(C12)</f>
+        <v>studenten, docenten kunnen projectdetails opvragen</v>
+      </c>
+      <c r="J12" s="15" t="str">
+        <f>IF(LEFT(I12,1)=",",MID(I12,3,LEN(I12)),I12)</f>
+        <v>studenten, docenten kunnen projectdetails opvragen</v>
+      </c>
+      <c r="K12" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>Studenten, docenten kunnen projectdetails opvragen</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
@@ -973,21 +953,21 @@
         <v>5</v>
       </c>
       <c r="F13" s="6"/>
-      <c r="H13" s="22">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="I13" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v>studenten, docenten, gasten kunnen projecten delen op sociale media</v>
-      </c>
-      <c r="J13" s="15" t="str">
-        <f t="shared" si="4"/>
-        <v>studenten, docenten, gasten kunnen projecten delen op sociale media</v>
-      </c>
-      <c r="K13" s="16" t="str">
-        <f t="shared" si="3"/>
-        <v>Studenten, docenten, gasten kunnen projecten delen op sociale media</v>
+      <c r="H13" s="11">
+        <f>B13</f>
+        <v>8</v>
+      </c>
+      <c r="I13" s="19" t="str">
+        <f>IF(D13="x",LOWER($D$5),"")&amp;IF(E13="x",", " &amp; LOWER($E$5),"")&amp;IF(F13="x", ", " &amp; LOWER($F$5),"") &amp; " kunnen " &amp; LOWER(C13)</f>
+        <v>studenten, docenten kunnen projectnieuws bekijken</v>
+      </c>
+      <c r="J13" s="19" t="str">
+        <f t="shared" ref="J13:J14" si="2">IF(LEFT(I13,1)=",",MID(I13,3,LEN(I13)),I13)</f>
+        <v>studenten, docenten kunnen projectnieuws bekijken</v>
+      </c>
+      <c r="K13" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Studenten, docenten kunnen projectnieuws bekijken</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
@@ -1006,21 +986,21 @@
       <c r="F14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="11">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I14" s="19" t="str">
-        <f t="shared" si="1"/>
-        <v>studenten kunnen inschrijven op projecten</v>
-      </c>
-      <c r="J14" s="19" t="str">
-        <f t="shared" ref="J14:J20" si="5">IF(LEFT(I14,1)=",",MID(I14,3,LEN(I14)),I14)</f>
-        <v>studenten kunnen inschrijven op projecten</v>
-      </c>
-      <c r="K14" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v>Studenten kunnen inschrijven op projecten</v>
+      <c r="H14" s="22">
+        <f>B14</f>
+        <v>9</v>
+      </c>
+      <c r="I14" s="15" t="str">
+        <f>IF(D14="x",LOWER($D$5),"")&amp;IF(E14="x",", " &amp; LOWER($E$5),"")&amp;IF(F14="x", ", " &amp; LOWER($F$5),"") &amp; " kunnen " &amp; LOWER(C14)</f>
+        <v>studenten, docenten, gasten kunnen projecten delen op sociale media</v>
+      </c>
+      <c r="J14" s="15" t="str">
+        <f t="shared" si="2"/>
+        <v>studenten, docenten, gasten kunnen projecten delen op sociale media</v>
+      </c>
+      <c r="K14" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>Studenten, docenten, gasten kunnen projecten delen op sociale media</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
@@ -1035,21 +1015,21 @@
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="6"/>
-      <c r="H15" s="22">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="I15" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v>studenten, docenten kunnen projecten bewerken</v>
-      </c>
-      <c r="J15" s="15" t="str">
-        <f t="shared" si="5"/>
-        <v>studenten, docenten kunnen projecten bewerken</v>
-      </c>
-      <c r="K15" s="16" t="str">
-        <f t="shared" si="3"/>
-        <v>Studenten, docenten kunnen projecten bewerken</v>
+      <c r="H15" s="11">
+        <f>B15</f>
+        <v>10</v>
+      </c>
+      <c r="I15" s="19" t="str">
+        <f>IF(D15="x",LOWER($D$5),"")&amp;IF(E15="x",", " &amp; LOWER($E$5),"")&amp;IF(F15="x", ", " &amp; LOWER($F$5),"") &amp; " kunnen " &amp; LOWER(C15)</f>
+        <v>studenten kunnen inschrijven op projecten</v>
+      </c>
+      <c r="J15" s="19" t="str">
+        <f t="shared" ref="J15:J21" si="3">IF(LEFT(I15,1)=",",MID(I15,3,LEN(I15)),I15)</f>
+        <v>studenten kunnen inschrijven op projecten</v>
+      </c>
+      <c r="K15" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Studenten kunnen inschrijven op projecten</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
@@ -1066,21 +1046,21 @@
         <v>5</v>
       </c>
       <c r="F16" s="2"/>
-      <c r="H16" s="11">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="I16" s="19" t="str">
-        <f t="shared" si="1"/>
-        <v>studenten, docenten kunnen projecten verwijderen</v>
-      </c>
-      <c r="J16" s="19" t="str">
-        <f t="shared" si="5"/>
-        <v>studenten, docenten kunnen projecten verwijderen</v>
-      </c>
-      <c r="K16" s="20" t="str">
+      <c r="H16" s="22">
+        <f>B16</f>
+        <v>11</v>
+      </c>
+      <c r="I16" s="15" t="str">
+        <f>IF(D16="x",LOWER($D$5),"")&amp;IF(E16="x",", " &amp; LOWER($E$5),"")&amp;IF(F16="x", ", " &amp; LOWER($F$5),"") &amp; " kunnen " &amp; LOWER(C16)</f>
+        <v>studenten, docenten kunnen projecten bewerken</v>
+      </c>
+      <c r="J16" s="15" t="str">
         <f t="shared" si="3"/>
-        <v>Studenten, docenten kunnen projecten verwijderen</v>
+        <v>studenten, docenten kunnen projecten bewerken</v>
+      </c>
+      <c r="K16" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>Studenten, docenten kunnen projecten bewerken</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
@@ -1097,21 +1077,21 @@
         <v>5</v>
       </c>
       <c r="F17" s="6"/>
-      <c r="H17" s="22">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="I17" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v>studenten kunnen annountsments aanmaken</v>
-      </c>
-      <c r="J17" s="15" t="str">
-        <f t="shared" si="5"/>
-        <v>studenten kunnen annountsments aanmaken</v>
-      </c>
-      <c r="K17" s="16" t="str">
-        <f>UPPER(LEFT(J17,1))&amp;LOWER(RIGHT(J17,LEN(J17)-1))</f>
-        <v>Studenten kunnen annountsments aanmaken</v>
+      <c r="H17" s="11">
+        <f>B17</f>
+        <v>12</v>
+      </c>
+      <c r="I17" s="19" t="str">
+        <f>IF(D17="x",LOWER($D$5),"")&amp;IF(E17="x",", " &amp; LOWER($E$5),"")&amp;IF(F17="x", ", " &amp; LOWER($F$5),"") &amp; " kunnen " &amp; LOWER(C17)</f>
+        <v>studenten, docenten kunnen projecten verwijderen</v>
+      </c>
+      <c r="J17" s="19" t="str">
+        <f t="shared" si="3"/>
+        <v>studenten, docenten kunnen projecten verwijderen</v>
+      </c>
+      <c r="K17" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Studenten, docenten kunnen projecten verwijderen</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -1126,21 +1106,21 @@
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="2"/>
-      <c r="H18" s="11">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="I18" s="19" t="str">
-        <f t="shared" si="1"/>
-        <v>studenten kunnen projecten aanmaken</v>
-      </c>
-      <c r="J18" s="19" t="str">
-        <f t="shared" si="5"/>
-        <v>studenten kunnen projecten aanmaken</v>
-      </c>
-      <c r="K18" s="20" t="str">
+      <c r="H18" s="22">
+        <f>B18</f>
+        <v>13</v>
+      </c>
+      <c r="I18" s="15" t="str">
+        <f>IF(D18="x",LOWER($D$5),"")&amp;IF(E18="x",", " &amp; LOWER($E$5),"")&amp;IF(F18="x", ", " &amp; LOWER($F$5),"") &amp; " kunnen " &amp; LOWER(C18)</f>
+        <v>studenten kunnen annountsments aanmaken</v>
+      </c>
+      <c r="J18" s="15" t="str">
         <f t="shared" si="3"/>
-        <v>Studenten kunnen projecten aanmaken</v>
+        <v>studenten kunnen annountsments aanmaken</v>
+      </c>
+      <c r="K18" s="16" t="str">
+        <f>UPPER(LEFT(J18,1))&amp;LOWER(RIGHT(J18,LEN(J18)-1))</f>
+        <v>Studenten kunnen annountsments aanmaken</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -1155,21 +1135,21 @@
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="6"/>
-      <c r="H19" s="22">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="I19" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v>studenten kunnen milestone-statussen aanpassen</v>
-      </c>
-      <c r="J19" s="15" t="str">
-        <f t="shared" si="5"/>
-        <v>studenten kunnen milestone-statussen aanpassen</v>
-      </c>
-      <c r="K19" s="16" t="str">
+      <c r="H19" s="11">
+        <f>B19</f>
+        <v>14</v>
+      </c>
+      <c r="I19" s="19" t="str">
+        <f>IF(D19="x",LOWER($D$5),"")&amp;IF(E19="x",", " &amp; LOWER($E$5),"")&amp;IF(F19="x", ", " &amp; LOWER($F$5),"") &amp; " kunnen " &amp; LOWER(C19)</f>
+        <v>studenten kunnen projecten aanmaken</v>
+      </c>
+      <c r="J19" s="19" t="str">
         <f t="shared" si="3"/>
-        <v>Studenten kunnen milestone-statussen aanpassen</v>
+        <v>studenten kunnen projecten aanmaken</v>
+      </c>
+      <c r="K19" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Studenten kunnen projecten aanmaken</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
@@ -1184,21 +1164,21 @@
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="2"/>
-      <c r="H20" s="11">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="I20" s="19" t="str">
-        <f t="shared" si="1"/>
-        <v>, docenten kunnen categorieen definieren</v>
-      </c>
-      <c r="J20" s="19" t="str">
-        <f t="shared" si="5"/>
-        <v>docenten kunnen categorieen definieren</v>
-      </c>
-      <c r="K20" s="20" t="str">
+      <c r="H20" s="22">
+        <f>B20</f>
+        <v>15</v>
+      </c>
+      <c r="I20" s="15" t="str">
+        <f>IF(D20="x",LOWER($D$5),"")&amp;IF(E20="x",", " &amp; LOWER($E$5),"")&amp;IF(F20="x", ", " &amp; LOWER($F$5),"") &amp; " kunnen " &amp; LOWER(C20)</f>
+        <v>studenten kunnen milestone-statussen aanpassen</v>
+      </c>
+      <c r="J20" s="15" t="str">
         <f t="shared" si="3"/>
-        <v>Docenten kunnen categorieen definieren</v>
+        <v>studenten kunnen milestone-statussen aanpassen</v>
+      </c>
+      <c r="K20" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>Studenten kunnen milestone-statussen aanpassen</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
@@ -1213,21 +1193,21 @@
         <v>5</v>
       </c>
       <c r="F21" s="6"/>
-      <c r="H21" s="22">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="I21" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v>, docenten kunnen projecten backen</v>
-      </c>
-      <c r="J21" s="15" t="str">
-        <f>IF(LEFT(I21,1)=",",MID(I21,3,LEN(I21)),I21)</f>
-        <v>docenten kunnen projecten backen</v>
-      </c>
-      <c r="K21" s="16" t="str">
+      <c r="H21" s="11">
+        <f>B21</f>
+        <v>16</v>
+      </c>
+      <c r="I21" s="19" t="str">
+        <f>IF(D21="x",LOWER($D$5),"")&amp;IF(E21="x",", " &amp; LOWER($E$5),"")&amp;IF(F21="x", ", " &amp; LOWER($F$5),"") &amp; " kunnen " &amp; LOWER(C21)</f>
+        <v>, docenten kunnen categorieen definieren</v>
+      </c>
+      <c r="J21" s="19" t="str">
         <f t="shared" si="3"/>
-        <v>Docenten kunnen projecten backen</v>
+        <v>docenten kunnen categorieen definieren</v>
+      </c>
+      <c r="K21" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Docenten kunnen categorieen definieren</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
@@ -1242,24 +1222,24 @@
         <v>5</v>
       </c>
       <c r="F22" s="2"/>
-      <c r="H22" s="11">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="I22" s="19" t="str">
-        <f t="shared" si="1"/>
-        <v>, docenten kunnen projecten publiek maken</v>
-      </c>
-      <c r="J22" s="19" t="str">
-        <f t="shared" ref="J22:J23" si="6">IF(LEFT(I22,1)=",",MID(I22,3,LEN(I22)),I22)</f>
-        <v>docenten kunnen projecten publiek maken</v>
-      </c>
-      <c r="K22" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v>Docenten kunnen projecten publiek maken</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H22" s="22">
+        <f>B22</f>
+        <v>17</v>
+      </c>
+      <c r="I22" s="15" t="str">
+        <f>IF(D22="x",LOWER($D$5),"")&amp;IF(E22="x",", " &amp; LOWER($E$5),"")&amp;IF(F22="x", ", " &amp; LOWER($F$5),"") &amp; " kunnen " &amp; LOWER(C22)</f>
+        <v>, docenten kunnen projecten backen</v>
+      </c>
+      <c r="J22" s="15" t="str">
+        <f>IF(LEFT(I22,1)=",",MID(I22,3,LEN(I22)),I22)</f>
+        <v>docenten kunnen projecten backen</v>
+      </c>
+      <c r="K22" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>Docenten kunnen projecten backen</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="5">
         <v>18</v>
       </c>
@@ -1271,21 +1251,21 @@
         <v>5</v>
       </c>
       <c r="F23" s="6"/>
-      <c r="H23" s="23">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="I23" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>, docenten kunnen inschrijvingen verwijderen</v>
-      </c>
-      <c r="J23" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v>docenten kunnen inschrijvingen verwijderen</v>
-      </c>
-      <c r="K23" s="18" t="str">
-        <f t="shared" si="3"/>
-        <v>Docenten kunnen inschrijvingen verwijderen</v>
+      <c r="H23" s="11">
+        <f>B23</f>
+        <v>18</v>
+      </c>
+      <c r="I23" s="19" t="str">
+        <f>IF(D23="x",LOWER($D$5),"")&amp;IF(E23="x",", " &amp; LOWER($E$5),"")&amp;IF(F23="x", ", " &amp; LOWER($F$5),"") &amp; " kunnen " &amp; LOWER(C23)</f>
+        <v>, docenten kunnen projecten publiek maken</v>
+      </c>
+      <c r="J23" s="19" t="str">
+        <f t="shared" ref="J23:J24" si="4">IF(LEFT(I23,1)=",",MID(I23,3,LEN(I23)),I23)</f>
+        <v>docenten kunnen projecten publiek maken</v>
+      </c>
+      <c r="K23" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Docenten kunnen projecten publiek maken</v>
       </c>
     </row>
     <row r="24" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1300,6 +1280,22 @@
         <v>5</v>
       </c>
       <c r="F24" s="4"/>
+      <c r="H24" s="23">
+        <f>B24</f>
+        <v>19</v>
+      </c>
+      <c r="I24" s="17" t="str">
+        <f>IF(D24="x",LOWER($D$5),"")&amp;IF(E24="x",", " &amp; LOWER($E$5),"")&amp;IF(F24="x", ", " &amp; LOWER($F$5),"") &amp; " kunnen " &amp; LOWER(C24)</f>
+        <v>, docenten kunnen inschrijvingen verwijderen</v>
+      </c>
+      <c r="J24" s="17" t="str">
+        <f t="shared" si="4"/>
+        <v>docenten kunnen inschrijvingen verwijderen</v>
+      </c>
+      <c r="K24" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>Docenten kunnen inschrijvingen verwijderen</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>